<commit_message>
Adding all changes \r\n To prove multiline from CMD
</commit_message>
<xml_diff>
--- a/COVID_19_tracker/EGY_COVID_19_Database.xlsx
+++ b/COVID_19_tracker/EGY_COVID_19_Database.xlsx
@@ -348,10 +348,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -430,31 +430,61 @@
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>2020-04-03 07:43:08.308140</t>
+          <t>2020-04-03 11:46:16.885835</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>865</v>
+        <v>985</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2020-04-03 08:16:52.323186</t>
+          <t>2020-04-04 14:59:10.656771</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>865</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2020-04-03 08:22:23.418639</t>
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>2020-04-05 11:37:24.874585</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>865</v>
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2020-04-06 14:01:22.145288</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>2020-04-10 12:22:18.681600</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2020-04-15 17:55:35.226085</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>